<commit_message>
doc - results for ridge regression and random forest
</commit_message>
<xml_diff>
--- a/final_project/results/selected_features.xlsx
+++ b/final_project/results/selected_features.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,17 +451,17 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>rfe</t>
+          <t>rfe_corr</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>mutual information</t>
+          <t>mutual information_corr</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>random forest</t>
+          <t>random forest_corr</t>
         </is>
       </c>
     </row>
@@ -510,22 +510,22 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Bottom-Vent-Yes-No</t>
+          <t>Pre-Test-Cell-Open-Circuit-Voltage-V</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>Pre-Test-Cell-Open-Circuit-Voltage-V</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>Pre-Test-Cell-Mass-g</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Pre-Test-Cell-Mass-g</t>
-        </is>
-      </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Bottom-Vent-Yes-No</t>
+          <t>Pre-Test-Cell-Open-Circuit-Voltage-V</t>
         </is>
       </c>
     </row>
@@ -542,184 +542,292 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Cell-Energy-Wh</t>
+          <t>Bottom-Vent-Yes-No</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Trigger-Mechanism_Nail</t>
+          <t>Pre-Test-Cell-Mass-g</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Cell-Nominal-Voltage-V</t>
+          <t>Pre-Test-Cell-Open-Circuit-Voltage-V</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Cell-Capacity-Ah</t>
+          <t>Bottom-Vent-Yes-No</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>State-of-Charge</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Pre-Test-Cell-Open-Circuit-Voltage-V</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>State-of-Charge</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>Trigger-Mechanism_Nail</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>Cell-Nominal-Voltage-V</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Trigger-Mechanism_Nail</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Chemistry_NMC/Graphite</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Bottom-Vent-Yes-No</t>
-        </is>
-      </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Trigger-Mechanism_Nail</t>
+          <t>Cell-Capacity-Ah</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>Trigger-Mechanism_Nail</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>State-of-Charge</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Cell-Energy-Wh</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>Chemistry_NCA/Graphite</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>Bottom-Vent-Yes-No</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Cell-Capacity-Ah</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Pressure-Assisted-Seal-Configuration-Negative</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Chemistry_NMC/Graphite</t>
-        </is>
-      </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Cell-Nominal-Voltage-V</t>
+          <t>Trigger-Mechanism_Nail</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Pressure-Assisted-Seal-Configuration-Negative</t>
+          <t>Chemistry_NCA/Graphite</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>Cell-Nominal-Voltage-V</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Cell-Capacity-Ah</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>Chemistry_NMC/Graphite</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Chemistry_NMC/Graphite</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
         <is>
           <t>Cell-Nominal-Voltage-V</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Bottom-Vent-Yes-No</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Trigger-Mechanism_Nail</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Trigger-Mechanism_Heater (Non-ISC)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>Pressure-Assisted-Seal-Configuration-Negative</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>Bottom-Vent-Yes-No</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>Trigger-Mechanism_Nail</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Pressure-Assisted-Seal-Configuration-Negative</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Trigger-Mechanism_Nail</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Pressure-Assisted-Seal-Configuration-Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Bottom-Vent-Yes-No</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Chemistry_NMC/Graphite</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Cell-Nominal-Voltage-V</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Bottom-Vent-Yes-No</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Chemistry_NCA/Graphite</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
         <is>
           <t>Trigger-Mechanism_Heater (Non-ISC)</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Pressure-Assisted-Seal-Configuration-Positive</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr"/>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Pressure-Assisted-Seal-Configuration-Positive</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Pressure-Assisted-Seal-Configuration-Negative</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Trigger-Mechanism_Nail</t>
+        </is>
+      </c>
       <c r="C10" t="inlineStr">
         <is>
+          <t>Pressure-Assisted-Seal-Configuration-Positive</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Trigger-Mechanism_Heater (Non-ISC)</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
           <t>Pressure-Assisted-Seal-Configuration-Negative</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Chemistry_NCA/Graphite</t>
+        </is>
+      </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>Trigger-Mechanism_Heater (Non-ISC)</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Trigger-Mechanism_Heater (ISC)</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Trigger-Mechanism_Heater (Non-ISC)</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Pressure-Assisted-Seal-Configuration-Negative</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Pressure-Assisted-Seal-Configuration-Positive</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Trigger-Mechanism_Heater (ISC)</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
           <t>Chemistry_NCA/Graphite</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Pressure-Assisted-Seal-Configuration-Negative</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Pressure-Assisted-Seal-Configuration-Positive</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Pressure-Assisted-Seal-Configuration-Negative</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
doc - results ridge, rf, and mlp
</commit_message>
<xml_diff>
--- a/final_project/results/selected_features.xlsx
+++ b/final_project/results/selected_features.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -616,7 +616,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Bottom-Vent-Yes-No</t>
+          <t>Chemistry_NMC/Graphite</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -638,7 +638,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Cell-Capacity-Ah</t>
+          <t>Trigger-Mechanism_Nail</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -648,7 +648,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Chemistry_NMC/Graphite</t>
+          <t>Bottom-Vent-Yes-No</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -660,7 +660,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Pressure-Assisted-Seal-Configuration-Negative</t>
+          <t>Chemistry_NMC/Graphite</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -670,22 +670,22 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>Cell-Capacity-Ah</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Chemistry_NMC/Graphite-SiOx</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>Trigger-Mechanism_Nail</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Pressure-Assisted-Seal-Configuration-Negative</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Trigger-Mechanism_Nail</t>
-        </is>
-      </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Pressure-Assisted-Seal-Configuration-Positive</t>
+          <t>Trigger-Mechanism_Heater (Non-ISC)</t>
         </is>
       </c>
     </row>
@@ -710,14 +710,10 @@
           <t>Bottom-Vent-Yes-No</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Chemistry_NCA/Graphite</t>
-        </is>
-      </c>
+      <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Trigger-Mechanism_Heater (Non-ISC)</t>
+          <t>Chemistry_NMC/Graphite</t>
         </is>
       </c>
     </row>
@@ -730,104 +726,24 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Pressure-Assisted-Seal-Configuration-Positive</t>
+          <t>Trigger-Mechanism_Heater (Non-ISC)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Trigger-Mechanism_Heater (Non-ISC)</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Pressure-Assisted-Seal-Configuration-Negative</t>
-        </is>
-      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Chemistry_NCA/Graphite</t>
-        </is>
-      </c>
+      <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Trigger-Mechanism_Heater (Non-ISC)</t>
+          <t>Chemistry_NMC/Graphite</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Trigger-Mechanism_Heater (ISC)</t>
-        </is>
-      </c>
+      <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr"/>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Trigger-Mechanism_Heater (Non-ISC)</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Pressure-Assisted-Seal-Configuration-Negative</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Pressure-Assisted-Seal-Configuration-Positive</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Trigger-Mechanism_Heater (ISC)</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Chemistry_NCA/Graphite</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Pressure-Assisted-Seal-Configuration-Negative</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr"/>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Pressure-Assisted-Seal-Configuration-Positive</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr"/>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Pressure-Assisted-Seal-Configuration-Negative</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>